<commit_message>
Finalizado a estrutura do codigo
Concertar a questão da acentuação que o programa esta comendo
</commit_message>
<xml_diff>
--- a/arquivos/MAT.xlsx
+++ b/arquivos/MAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaob\Documents\GitHub\cartorio-automation\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCD193C-4E93-4A2E-983D-E71BB36CD1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D92950-6DFA-4822-A2D8-075AC2F803BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,29 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Registro n° R-1-5312, aos 20/11/82- Por escritura pública de compra e venda lavrada pelo Tabelião Substituto João Alves Martins, do 1° Oficio desta comarca, em data de 19/11/82, no livro n° 114, folhas 192 á 196, foi a parte de terra acima descrita, pela quantia de Cr$ 70.000,00 (setenta mil cruzeiros) adquirida pelo mesmo: LUIZ PEDRO DE MOURA, brasileiro, casado, trabalhador rural, domiciliado e residente neste Município, portador do CPF n° 390.935.654-00, figurando como transmitentes vendedor: Manoel Gonçalo de Lima, brasileiro, solteiro, maior, trabalhador rural, domiciliado e residente neste Município, portador do CPF n° 358.727.484-34. O Oficial Substituto: João Alves Martins.</t>
   </si>
   <si>
-    <t>Registro n° R-2-5312, aos 15/03/95- Em hipoteca especial de segundo grau, sem concorrência de terceiros, foi dado o imóvel acima descrito em garantia do financiamento de R$ 2.193,00, deferido pela CRH n° FIR-95/017-7, datado de 15/05/95, com vencimento para 15/10/1999, juros e formas de pagamento descritos no mesmo contrato, em favor do Banco do Nordeste do Brasil S/A, agencia local, CGC n° 07.237.3730111-64. Devedores: LUIZ PEDRO DE MOURA e sua esposa MARIA DO SOCORRO DE LIMA MOURA, brasileiros, casados, agricultores, residentes e domiciliados nesta cidade, portadores do CPF n° 390.935.654-00. O Oficial: João Alves Martins.</t>
-  </si>
-  <si>
-    <t>Registro n° R-3-5312, aos 15/03/95- Em hipoteca especial de primeiro grau e sem concorrência de terceiros, em favor do mesmo Banco, foi o mesmo imóvel em garantia do financiamento de R$ 8.780,00 (oito mil setecentos e oitenta reais); deferido pela CRPH n° FIR-95/018-5, com vencimento para 15/04/2007, datada de 15/03/95. Devedores: LUIZ PEDRO DE MOURA e sua esposa MARIA DO SOCORRO DE LIMA MOURA. O Oficial: João Alves Martins.</t>
-  </si>
-  <si>
-    <t>Registro n° R-4-5312, aos 15/09/2005- Em hipoteca especial de 2° grau e sem concorrência de terceiros, o imóvel acima descrito, em favor do Banco do Nordeste do Brasil S/A, agencia desta cidade, para garantia do financiamento de R$ 6.730,95, da divida liquida, deferido pela escritura pública de composição e confissão de dividas lavrada pelo Tabelião João Alves Martins, do 1° Oficio desta comarca, no livro n° 230, folhas 121/123, em data de 05/09/2005, com vencimento para 02/05/2015, com as condições, encargos, prazo e forma de pagamento descritos no mesmo instrumento. Devedor: LUIZ PEDRO DE MOURA, CPF n° 390.935.654-00 e sua esposa MARIA DO SOCORRO DE LIMA MOURA. O Oficial: João Alves Martins.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Averbação n° AV-5-5312, aos 27/07/2015- Por Baixa de Hipoteca emitido pelo Banco do Nordeste do Brasil S/A, em data de 06/06/2015, fica CANCELADO o ônus hipotecário do Registro n° R-2 supra. (TSNR-R$ 10,92 e FERC-R$ 5,47). Márcia Valéria Martins. </t>
   </si>
   <si>
-    <t>Averbação n° AV-6-5312, aos 27/07/2015- Por Baixa de Hipoteca emitido pelo Banco do Nordeste do Brasil S/A, em data de 06/06/2015, fica CANCELADO o ônus hipotecário do Registro n° R-3 supra. (TSNR-R$ 10,92 e FERC-R$ 5,47). Márcia Valéria Martins.</t>
-  </si>
-  <si>
-    <t>Averbação n° AV-7-5312, aos 27/07/2015- Por Baixa de Hipoteca emitido pelo Banco do Nordeste do Brasil S/A, em data de 06/06/2015, fica CANCELADO o ônus hipotecário do Registro n° R-4 supra. (TSNR-R$ 10,92 e FERC-R$ 5,47). Márcia Valéria Martins.</t>
-  </si>
-  <si>
     <t>AVERBAÇÃO Nº. AV-8 - 5312, AOS 18/09/2015 - Por escritura pública de compra e venda foi desmembrado do imóvel supra uma faixa de terrea medindo 44,00m x 2.420,00m, área total de 10,64ha, para Francisco Duarte de Lima e passou a ser objeto do R-1, da matricula nº. 25.627, ficha 01 do Livro 2 de Registro Geral. (TSNR R$ 10,92 e FERC R$ 5,47). Área remanescente 28,96ha (vinte e oito hectares e noventa e seis centesimos).</t>
   </si>
   <si>
@@ -61,13 +46,22 @@
   </si>
   <si>
     <t>CONTADOR</t>
+  </si>
+  <si>
+    <t>20/08/1925</t>
+  </si>
+  <si>
+    <t>20/08/1929</t>
+  </si>
+  <si>
+    <t>20/08/1932</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +74,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,13 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,147 +388,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="73.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="73.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>30275</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>34773</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>34773</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>38487</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>42212</v>
-      </c>
-      <c r="B6" s="3">
-        <v>5</v>
-      </c>
-      <c r="C6">
+      <c r="D4" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>42212</v>
-      </c>
-      <c r="B7" s="3">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>42212</v>
-      </c>
-      <c r="B8" s="3">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>42265</v>
-      </c>
-      <c r="B9" s="3">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
atualizado o pip e corrigido o erro dos acentos
</commit_message>
<xml_diff>
--- a/arquivos/MAT.xlsx
+++ b/arquivos/MAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaob\Documents\GitHub\cartorio-automation\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D92950-6DFA-4822-A2D8-075AC2F803BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6D1CF8-70A1-407D-A435-53B1759B1C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Registro n° R-1-5312, aos 20/11/82- Por escritura pública de compra e venda lavrada pelo Tabelião Substituto João Alves Martins, do 1° Oficio desta comarca, em data de 19/11/82, no livro n° 114, folhas 192 á 196, foi a parte de terra acima descrita, pela quantia de Cr$ 70.000,00 (setenta mil cruzeiros) adquirida pelo mesmo: LUIZ PEDRO DE MOURA, brasileiro, casado, trabalhador rural, domiciliado e residente neste Município, portador do CPF n° 390.935.654-00, figurando como transmitentes vendedor: Manoel Gonçalo de Lima, brasileiro, solteiro, maior, trabalhador rural, domiciliado e residente neste Município, portador do CPF n° 358.727.484-34. O Oficial Substituto: João Alves Martins.</t>
   </si>
@@ -39,9 +39,6 @@
     <t>DATA</t>
   </si>
   <si>
-    <t>TIPO</t>
-  </si>
-  <si>
     <t>TEXTO</t>
   </si>
   <si>
@@ -55,6 +52,18 @@
   </si>
   <si>
     <t>20/08/1932</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>x'x'</t>
   </si>
 </sst>
 </file>
@@ -391,7 +400,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H16" sqref="G15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,21 +417,21 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -433,10 +442,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -447,10 +456,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1">
         <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -463,5 +472,8 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:B4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>